<commit_message>
fix CSEI93 source codes
</commit_message>
<xml_diff>
--- a/scoring/tests/CSEI/CSEI93_test_1.xlsx
+++ b/scoring/tests/CSEI/CSEI93_test_1.xlsx
@@ -450,7 +450,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">

</xml_diff>